<commit_message>
added codes, dummys for pcl segment
</commit_message>
<xml_diff>
--- a/auswertung_disparity.xlsx
+++ b/auswertung_disparity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Masterarbeit\Stereomatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C2DA2C-DCE3-404E-B1FD-EBDF3AB9F512}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5E0360-9AAA-4011-BAAA-C0231FC4EB1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{9F09BA9E-D75F-4560-BEC7-C3CEA781B600}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>OpenCV Blockmatch</t>
   </si>
@@ -216,6 +216,27 @@
   </si>
   <si>
     <t>601s</t>
+  </si>
+  <si>
+    <t>Custom Diff</t>
+  </si>
+  <si>
+    <t>1147s</t>
+  </si>
+  <si>
+    <t>2343s</t>
+  </si>
+  <si>
+    <t>3678s</t>
+  </si>
+  <si>
+    <t>4955s</t>
+  </si>
+  <si>
+    <t>6821s</t>
+  </si>
+  <si>
+    <t>0.057</t>
   </si>
 </sst>
 </file>
@@ -569,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4209DCCE-11B1-4B5F-B861-EBB3B8002F5E}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +1015,62 @@
         <v>59</v>
       </c>
     </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.434</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>